<commit_message>
update for text xml string
</commit_message>
<xml_diff>
--- a/Data Files/TC-02/2-2.xlsx
+++ b/Data Files/TC-02/2-2.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="100" iterateDelta="0.001"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -63,7 +63,14 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,157 +526,157 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -994,13 +1001,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
-  <cols>
-    <col min="1" max="1" width="20.3333333333333" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">

</xml_diff>